<commit_message>
Homework 3 ver 1 | Homework 2 update
</commit_message>
<xml_diff>
--- a/20220312/Instruction_2100011047_.xlsx
+++ b/20220312/Instruction_2100011047_.xlsx
@@ -2239,51 +2239,51 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>jne</t>
+          <t>setae</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>paddq</t>
+          <t>shlq</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lahf</t>
+          <t>frndint</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>shrdq</t>
+          <t>pshufd</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>decw</t>
+          <t>jmp</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2293,200 +2293,200 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>frndint</t>
+          <t>cli</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>pshufd</t>
+          <t>jmp</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>nopl</t>
+          <t>negl</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>divsd</t>
+          <t>cmovbq</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>cwtl</t>
+          <t>retq</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>shldq</t>
+          <t>rep</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>setae</t>
+          <t>nopl</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cmovbq</t>
+          <t>btq</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>cli</t>
+          <t>cld</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>jmp</t>
+          <t>shldq</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>jo</t>
+          <t>setns</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cmovgel</t>
+          <t>xaddl</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>std</t>
+          <t>lock</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>imull</t>
+          <t>callq</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>jae</t>
+          <t>sarq</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>cmpxchgl</t>
+          <t>testl</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>cltd</t>
+          <t>std</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>rep</t>
+          <t>imull</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>setns</t>
+          <t>decw</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cvtss2sd</t>
+          <t>movsd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>sahf</t>
+          <t>cltd</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>callq</t>
+          <t>shrdq</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>sarq</t>
+          <t>notl</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cmovlq</t>
+          <t>xorps</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>retq</t>
+          <t>ud2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>imulq</t>
+          <t>.byte</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>popq</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>cmovgel</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>lahf</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>imulq</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>testw</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sti</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>.byte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>jl</t>
+          <t>seto</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>movzwl</t>
+          <t>cmovbel</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>cld</t>
+          <t>sahf</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>je</t>
+          <t>incl</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>jmp</t>
+          <t>shrl</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>nop</t>
+          <t>cwtl</t>
         </is>
       </c>
     </row>
@@ -2498,58 +2498,58 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>cmovnew</t>
+          <t>movq</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ud2</t>
+          <t>cltq</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>divq</t>
+          <t>jb</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>psrlq</t>
+          <t>movups</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>lock</t>
+          <t>nop</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>jns</t>
+          <t>jo</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>movb</t>
+          <t>xaddq</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>cltq</t>
+          <t>sti</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ljmpl</t>
+          <t>decl</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>movups</t>
+          <t>cmovneq</t>
         </is>
       </c>
     </row>
@@ -2561,769 +2561,769 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>cmovael</t>
+          <t>movl</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>lcalll</t>
+          <t>pushq</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>movaps</t>
+          <t>movapd</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>jmp</t>
+          <t>nopw</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>cmovgq</t>
+          <t>subsd</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>callq</t>
+          <t>jl</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>testq</t>
+          <t>divsd</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>jb</t>
+          <t>jle</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>movsbl</t>
+          <t>cmpb</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>jbe</t>
+          <t>js</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>addw</t>
+          <t>cmovael</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>setge</t>
+          <t>jae</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>xaddl</t>
+          <t>cmovel</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>shrq</t>
+          <t>jg</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>shlb</t>
+          <t>jmp</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>negq</t>
+          <t>jns</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>pxor</t>
+          <t>subl</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>idivl</t>
+          <t>jmpq</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>cmovbl</t>
+          <t>addb</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>nopw</t>
+          <t>sete</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cvtsd2ss</t>
+          <t>cvtsi2sdq</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>setbe</t>
+          <t>divq</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>cmpl</t>
+          <t>cmovgew</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>jno</t>
+          <t>shrl</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>sarl</t>
+          <t>imull</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>shrl</t>
+          <t>setl</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>orq</t>
+          <t>por</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>popq</t>
+          <t>idivl</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>punpcklqdq</t>
+          <t>cmovnew</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>incq</t>
+          <t>ja</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>leal</t>
+          <t>ucomisd</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>setg</t>
+          <t>decb</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>movl</t>
+          <t>orb</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>mulq</t>
+          <t>setg</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>cmovgl</t>
+          <t>adcq</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>shrb</t>
+          <t>imulq</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>movdqu</t>
+          <t>shlb</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>seto</t>
+          <t>setbe</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>adcq</t>
+          <t>movdqu</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>seta</t>
+          <t>setge</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>xorl</t>
+          <t>cmpw</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>pushq</t>
+          <t>mulq</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>cmpw</t>
+          <t>movzwl</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>decl</t>
+          <t>callq</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>cmovaeq</t>
+          <t>maxsd</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>setl</t>
+          <t>negq</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>cmovnel</t>
+          <t>testw</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>decb</t>
+          <t>jno</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>cmovneq</t>
+          <t>cvtss2sd</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>incl</t>
+          <t>setb</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>cmovbeq</t>
+          <t>movdqa</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>notl</t>
+          <t>incb</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>movsbq</t>
+          <t>shrq</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>jg</t>
+          <t>je</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>xaddq</t>
+          <t>andq</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>negl</t>
+          <t>setne</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>orb</t>
+          <t>cmpl</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>setne</t>
+          <t>jne</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>subl</t>
+          <t>cmpxchgl</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>jmpq</t>
+          <t>ljmpl</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>movw</t>
+          <t>addw</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ja</t>
+          <t>incq</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>movabsq</t>
+          <t>xorb</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>incb</t>
+          <t>shrb</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>subq</t>
+          <t>subb</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sets</t>
+          <t>shrq</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>movapd</t>
+          <t>shll</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>sete</t>
+          <t>fdivr</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ucomisd</t>
+          <t>movswl</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>fdivr</t>
+          <t>lcalll</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>mulsd</t>
+          <t>orl</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>setb</t>
+          <t>jbe</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>subb</t>
+          <t>movabsq</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>js</t>
+          <t>notq</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>xorpd</t>
+          <t>paddq</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>jle</t>
+          <t>seta</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>subsd</t>
+          <t>pxor</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>notq</t>
+          <t>sets</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>addl</t>
+          <t>punpcklqdq</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="inlineStr">
         <is>
-          <t>testb</t>
+          <t>cmovbl</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
         <is>
-          <t>addq</t>
+          <t>movsbl</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
         <is>
-          <t>cmovgew</t>
+          <t>leaq</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
         <is>
-          <t>imulq</t>
+          <t>cmovsq</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
         <is>
-          <t>orl</t>
+          <t>imulq</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
         <is>
-          <t>cmovel</t>
+          <t>leal</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
         <is>
-          <t>psllq</t>
+          <t>callq</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
         <is>
-          <t>shrq</t>
+          <t>cmovbeq</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
         <is>
-          <t>andb</t>
+          <t>orq</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="inlineStr">
         <is>
-          <t>shlq</t>
+          <t>xorq</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
         <is>
-          <t>cmpb</t>
+          <t>shrb</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
         <is>
-          <t>movsd</t>
+          <t>xorpd</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="inlineStr">
         <is>
-          <t>cmovnsq</t>
+          <t>cmovlq</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="inlineStr">
         <is>
-          <t>cmpq</t>
+          <t>cmovaq</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
         <is>
-          <t>cmoveq</t>
+          <t>movsbq</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
         <is>
-          <t>movdqa</t>
+          <t>andl</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
         <is>
-          <t>btq</t>
+          <t>sarq</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
         <is>
-          <t>xorps</t>
+          <t>addl</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
         <is>
-          <t>por</t>
+          <t>cmovnsq</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="inlineStr">
         <is>
-          <t>leaq</t>
+          <t>cvtsd2ss</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
         <is>
-          <t>andq</t>
+          <t>testq</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
         <is>
-          <t>testl</t>
+          <t>movb</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
         <is>
-          <t>cmovsq</t>
+          <t>cmovaeq</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="inlineStr">
         <is>
-          <t>sarq</t>
+          <t>psrlq</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
         <is>
-          <t>adcb</t>
+          <t>xorl</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
         <is>
-          <t>addb</t>
+          <t>movaps</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
         <is>
-          <t>xorq</t>
+          <t>movw</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
         <is>
-          <t>callq</t>
+          <t>adcb</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
         <is>
-          <t>movq</t>
+          <t>andb</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
         <is>
-          <t>andl</t>
+          <t>psllq</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
         <is>
-          <t>shrl</t>
+          <t>addsd</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
         <is>
-          <t>shrb</t>
+          <t>cmpq</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
         <is>
-          <t>movswl</t>
+          <t>cmoveq</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
         <is>
-          <t>xorb</t>
+          <t>cmovnel</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
         <is>
-          <t>shll</t>
+          <t>testb</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="inlineStr">
         <is>
-          <t>maxsd</t>
+          <t>movslq</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
         <is>
-          <t>movslq</t>
+          <t>addq</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
         <is>
-          <t>cmovbel</t>
+          <t>subq</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
         <is>
-          <t>imull</t>
+          <t>cmovgl</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
         <is>
-          <t>cmovaq</t>
+          <t>mulsd</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="inlineStr">
         <is>
-          <t>cvtsi2sdq</t>
+          <t>sarl</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="inlineStr">
         <is>
-          <t>addsd</t>
+          <t>cmovgq</t>
         </is>
       </c>
     </row>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3464,7 +3464,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3479,7 +3479,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3494,7 +3494,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3509,7 +3509,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3539,7 +3539,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3764,7 +3764,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4139,7 +4139,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4319,7 +4319,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4364,7 +4364,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -4619,7 +4619,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4874,7 +4874,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4934,7 +4934,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4964,7 +4964,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -4979,7 +4979,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5084,7 +5084,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5114,7 +5114,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5369,7 +5369,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5384,7 +5384,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
     </row>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5579,7 +5579,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5609,7 +5609,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5654,7 +5654,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5729,7 +5729,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5744,7 +5744,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5849,7 +5849,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5864,7 +5864,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5909,7 +5909,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5924,7 +5924,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
     </row>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
     </row>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
     </row>
@@ -6052,7 +6052,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0 Arguments</t>
+          <t>无参指令</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -6062,7 +6062,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1 Arguments</t>
+          <t>单参指令</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -6072,7 +6072,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2 Arguments</t>
+          <t>双参指令</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -6082,7 +6082,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3+ Arguments</t>
+          <t>多参指令</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>